<commit_message>
V0.5.0 Refactor module structure
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/eo.xlsx
+++ b/builder/src/main/resources/eo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werner.diwischek/dev/elasticobjects/builder/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD37945-4F35-3F4C-B078-91CE599614AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E676744-287C-7B45-8992-D46B59134C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" activeTab="2" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" activeTab="4" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="DbSqlConfig" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DbSqlConfig!$A$1:$J$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FieldConfig!$A$1:$I$122</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FileConfig!$A$1:$M$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ModelConfig!$A$1:$L$108</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="707">
   <si>
     <t>naturalId</t>
   </si>
@@ -2238,6 +2239,9 @@
   </si>
   <si>
     <t>faq</t>
+  </si>
+  <si>
+    <t>elastic-objects-test</t>
   </si>
 </sst>
 </file>
@@ -2623,13 +2627,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2949A4-7E1C-7F4B-A1BC-11445B521B01}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N108"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2694,7 +2699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>169</v>
       </c>
@@ -2727,8 +2732,8 @@
       <c r="A3" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
+      <c r="C3" t="s">
+        <v>706</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -2755,7 +2760,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -2781,7 +2786,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="177" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>174</v>
       </c>
@@ -2814,8 +2819,8 @@
       <c r="A6" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
+      <c r="C6" t="s">
+        <v>706</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -2842,7 +2847,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2868,7 +2873,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>177</v>
       </c>
@@ -2900,7 +2905,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="372" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="372" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>180</v>
       </c>
@@ -2935,7 +2940,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>182</v>
       </c>
@@ -2970,7 +2975,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>184</v>
       </c>
@@ -2999,7 +3004,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>185</v>
       </c>
@@ -3028,7 +3033,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>188</v>
       </c>
@@ -3063,7 +3068,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>290</v>
       </c>
@@ -3098,7 +3103,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>191</v>
       </c>
@@ -3133,7 +3138,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="255" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>195</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>194</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>628</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>198</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>200</v>
       </c>
@@ -3303,7 +3308,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>202</v>
       </c>
@@ -3335,7 +3340,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>204</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>462</v>
       </c>
@@ -3405,7 +3410,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>463</v>
       </c>
@@ -3437,7 +3442,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>467</v>
       </c>
@@ -3469,7 +3474,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -3495,7 +3500,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>293</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>297</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>299</v>
       </c>
@@ -3597,7 +3602,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>301</v>
       </c>
@@ -3629,7 +3634,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>303</v>
       </c>
@@ -3664,7 +3669,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>305</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>635</v>
       </c>
@@ -3729,7 +3734,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>633</v>
       </c>
@@ -3765,7 +3770,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>691</v>
       </c>
@@ -3798,7 +3803,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>154</v>
       </c>
@@ -3824,7 +3829,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>206</v>
       </c>
@@ -3856,7 +3861,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>208</v>
       </c>
@@ -3885,7 +3890,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
@@ -3917,7 +3922,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>211</v>
       </c>
@@ -3952,7 +3957,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>213</v>
       </c>
@@ -3987,7 +3992,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>215</v>
       </c>
@@ -4019,7 +4024,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>217</v>
       </c>
@@ -4054,7 +4059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>155</v>
       </c>
@@ -4080,7 +4085,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>629</v>
       </c>
@@ -4116,7 +4121,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
@@ -4145,7 +4150,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>219</v>
       </c>
@@ -4177,7 +4182,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>83</v>
       </c>
@@ -4203,7 +4208,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>221</v>
       </c>
@@ -4235,7 +4240,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>225</v>
       </c>
@@ -4270,7 +4275,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>142</v>
       </c>
@@ -4296,7 +4301,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -4328,7 +4333,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>230</v>
       </c>
@@ -4360,7 +4365,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>232</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>233</v>
       </c>
@@ -4418,7 +4423,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>234</v>
       </c>
@@ -4447,7 +4452,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>427</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
@@ -4511,7 +4516,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>238</v>
       </c>
@@ -4549,7 +4554,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>468</v>
       </c>
@@ -4584,7 +4589,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>102</v>
       </c>
@@ -4610,7 +4615,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>47</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>239</v>
       </c>
@@ -4659,7 +4664,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>686</v>
       </c>
@@ -4692,7 +4697,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>241</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>243</v>
       </c>
@@ -4759,7 +4764,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>245</v>
       </c>
@@ -4791,7 +4796,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>247</v>
       </c>
@@ -4823,7 +4828,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>249</v>
       </c>
@@ -4855,7 +4860,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>251</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>253</v>
       </c>
@@ -4919,7 +4924,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>685</v>
       </c>
@@ -4952,7 +4957,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>682</v>
       </c>
@@ -4988,7 +4993,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>255</v>
       </c>
@@ -5020,7 +5025,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>156</v>
       </c>
@@ -5049,7 +5054,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>66</v>
       </c>
@@ -5078,7 +5083,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>258</v>
       </c>
@@ -5110,7 +5115,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>260</v>
       </c>
@@ -5142,7 +5147,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>514</v>
       </c>
@@ -5178,7 +5183,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>513</v>
       </c>
@@ -5210,7 +5215,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>512</v>
       </c>
@@ -5242,7 +5247,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>547</v>
       </c>
@@ -5280,7 +5285,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>549</v>
       </c>
@@ -5316,7 +5321,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>133</v>
       </c>
@@ -5348,7 +5353,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>263</v>
       </c>
@@ -5380,7 +5385,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>265</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>267</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>269</v>
       </c>
@@ -5479,7 +5484,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>147</v>
       </c>
@@ -5511,7 +5516,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>271</v>
       </c>
@@ -5540,7 +5545,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>224</v>
       </c>
@@ -5572,7 +5577,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>273</v>
       </c>
@@ -5604,7 +5609,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>16</v>
       </c>
@@ -5630,7 +5635,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>275</v>
       </c>
@@ -5659,7 +5664,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>276</v>
       </c>
@@ -5688,7 +5693,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>277</v>
       </c>
@@ -5720,7 +5725,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>279</v>
       </c>
@@ -5755,7 +5760,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="125" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>562</v>
       </c>
@@ -5787,7 +5792,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>577</v>
       </c>
@@ -5819,7 +5824,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>281</v>
       </c>
@@ -5851,7 +5856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>283</v>
       </c>
@@ -5883,7 +5888,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>284</v>
       </c>
@@ -5918,7 +5923,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>286</v>
       </c>
@@ -5956,7 +5961,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>551</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>312</v>
       </c>
@@ -6030,7 +6035,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="118" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>288</v>
       </c>
@@ -6065,7 +6070,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>315</v>
       </c>
@@ -6103,7 +6108,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>318</v>
       </c>
@@ -6136,7 +6141,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L108" xr:uid="{54A0279D-8AE7-C14E-B9E3-5E0BAE0A3850}"/>
+  <autoFilter ref="A1:L108" xr:uid="{54A0279D-8AE7-C14E-B9E3-5E0BAE0A3850}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="eo-test"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:N108">
     <sortCondition ref="A2:A108"/>
   </sortState>
@@ -6147,6 +6158,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B963DEC-06FA-0F4E-B89A-363FE5F4C7EE}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J941"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6154,7 +6166,7 @@
       <selection activeCell="E15" sqref="E15"/>
       <selection pane="topRight" activeCell="E15" sqref="E15"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B99" sqref="B99:B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6201,7 +6213,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="86" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -6228,7 +6240,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="104" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -6263,7 +6275,7 @@
         <v>599</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -6286,7 +6298,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -6313,7 +6325,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>487</v>
       </c>
@@ -6343,7 +6355,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -6370,7 +6382,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6400,7 +6412,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6430,7 +6442,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -6460,7 +6472,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>405</v>
       </c>
@@ -6490,7 +6502,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -6520,7 +6532,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -6550,7 +6562,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -6580,7 +6592,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -6607,7 +6619,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>320</v>
       </c>
@@ -6634,7 +6646,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>322</v>
       </c>
@@ -6664,7 +6676,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>324</v>
       </c>
@@ -6691,7 +6703,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -6722,7 +6734,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -6752,7 +6764,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -6782,7 +6794,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>649</v>
       </c>
@@ -6812,7 +6824,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>326</v>
       </c>
@@ -6843,7 +6855,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -6870,7 +6882,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>559</v>
       </c>
@@ -6900,7 +6912,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -6928,7 +6940,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -6958,7 +6970,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -6986,7 +6998,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>327</v>
       </c>
@@ -7016,7 +7028,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -7046,7 +7058,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -7077,7 +7089,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -7104,7 +7116,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -7134,7 +7146,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -7164,7 +7176,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -7195,7 +7207,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -7226,7 +7238,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -7256,7 +7268,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -7286,7 +7298,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -7316,7 +7328,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>329</v>
       </c>
@@ -7346,7 +7358,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -7377,7 +7389,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -7404,7 +7416,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -7434,7 +7446,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -7464,7 +7476,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -7491,7 +7503,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -7521,7 +7533,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -7548,7 +7560,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -7578,7 +7590,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -7609,7 +7621,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>478</v>
       </c>
@@ -7636,7 +7648,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>331</v>
       </c>
@@ -7667,7 +7679,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -7698,7 +7710,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -7728,7 +7740,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -7756,7 +7768,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -7787,7 +7799,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -7815,7 +7827,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>98</v>
       </c>
@@ -7846,7 +7858,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>679</v>
       </c>
@@ -7877,7 +7889,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>460</v>
       </c>
@@ -7904,7 +7916,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -7933,7 +7945,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -7964,7 +7976,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>105</v>
       </c>
@@ -7994,7 +8006,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>107</v>
       </c>
@@ -8025,7 +8037,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -8055,7 +8067,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -8082,7 +8094,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -8112,7 +8124,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -8142,7 +8154,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>490</v>
       </c>
@@ -8172,7 +8184,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>114</v>
       </c>
@@ -8202,7 +8214,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -8229,7 +8241,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>117</v>
       </c>
@@ -8257,7 +8269,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>118</v>
       </c>
@@ -8285,7 +8297,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -8313,7 +8325,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>120</v>
       </c>
@@ -8343,7 +8355,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -8374,7 +8386,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>123</v>
       </c>
@@ -8404,7 +8416,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>125</v>
       </c>
@@ -8434,7 +8446,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -8463,7 +8475,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>676</v>
       </c>
@@ -8494,7 +8506,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>675</v>
       </c>
@@ -8525,7 +8537,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>489</v>
       </c>
@@ -8552,7 +8564,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>128</v>
       </c>
@@ -8583,7 +8595,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>129</v>
       </c>
@@ -8613,7 +8625,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>131</v>
       </c>
@@ -8644,7 +8656,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>132</v>
       </c>
@@ -8672,7 +8684,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>134</v>
       </c>
@@ -8702,7 +8714,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>136</v>
       </c>
@@ -8730,7 +8742,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>137</v>
       </c>
@@ -8758,7 +8770,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>138</v>
       </c>
@@ -8786,7 +8798,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>333</v>
       </c>
@@ -8816,7 +8828,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -8843,7 +8855,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>141</v>
       </c>
@@ -8870,7 +8882,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>144</v>
       </c>
@@ -8900,7 +8912,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>146</v>
       </c>
@@ -8928,7 +8940,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>335</v>
       </c>
@@ -8958,7 +8970,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>148</v>
       </c>
@@ -8988,7 +9000,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>337</v>
       </c>
@@ -9019,7 +9031,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>338</v>
       </c>
@@ -9051,7 +9063,7 @@
         <v>584</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C99" t="s">
         <v>12</v>
@@ -9079,8 +9091,8 @@
       <c r="A100" t="s">
         <v>585</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>18</v>
+      <c r="B100" t="s">
+        <v>706</v>
       </c>
       <c r="C100" t="s">
         <v>12</v>
@@ -9108,7 +9120,7 @@
         <v>586</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C101" t="s">
         <v>12</v>
@@ -9131,7 +9143,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>149</v>
       </c>
@@ -9161,7 +9173,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>151</v>
       </c>
@@ -9191,7 +9203,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>557</v>
       </c>
@@ -9221,7 +9233,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>153</v>
       </c>
@@ -9256,7 +9268,7 @@
         <v>587</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>
@@ -9285,7 +9297,7 @@
         <v>588</v>
       </c>
       <c r="B107" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C107" t="s">
         <v>12</v>
@@ -9314,7 +9326,7 @@
         <v>589</v>
       </c>
       <c r="B108" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C108" t="s">
         <v>12</v>
@@ -9343,7 +9355,7 @@
         <v>590</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C109" t="s">
         <v>12</v>
@@ -9372,7 +9384,7 @@
         <v>591</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C110" t="s">
         <v>12</v>
@@ -9400,7 +9412,7 @@
         <v>592</v>
       </c>
       <c r="B111" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C111" t="s">
         <v>12</v>
@@ -9429,7 +9441,7 @@
         <v>593</v>
       </c>
       <c r="B112" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C112" t="s">
         <v>12</v>
@@ -9457,7 +9469,7 @@
         <v>594</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C113" t="s">
         <v>12</v>
@@ -9483,7 +9495,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>159</v>
       </c>
@@ -9514,7 +9526,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>160</v>
       </c>
@@ -9547,7 +9559,7 @@
         <v>595</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C116" t="s">
         <v>12</v>
@@ -9576,7 +9588,7 @@
         <v>596</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
@@ -9599,7 +9611,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>161</v>
       </c>
@@ -9625,7 +9637,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>164</v>
       </c>
@@ -9655,7 +9667,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -9685,7 +9697,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>165</v>
       </c>
@@ -9714,7 +9726,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>167</v>
       </c>
@@ -10351,7 +10363,13 @@
       <c r="D941" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I122" xr:uid="{D69F739B-BFAA-8744-89E3-48A1C7C59643}"/>
+  <autoFilter ref="A1:I122" xr:uid="{D69F739B-BFAA-8744-89E3-48A1C7C59643}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="eo-test"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J122">
     <sortCondition ref="A2:A122"/>
   </sortState>
@@ -10364,12 +10382,12 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E15" sqref="E15"/>
       <selection pane="topRight" activeCell="E15" sqref="E15"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
-      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
+      <selection pane="bottomRight" activeCell="C57" sqref="C57:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10497,7 +10515,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>613</v>
       </c>
@@ -10535,7 +10553,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>615</v>
       </c>
@@ -10605,7 +10623,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>619</v>
       </c>
@@ -10808,7 +10826,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>376</v>
       </c>
@@ -10843,7 +10861,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>697</v>
       </c>
@@ -10878,7 +10896,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>378</v>
       </c>
@@ -10913,7 +10931,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>380</v>
       </c>
@@ -10948,7 +10966,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>544</v>
       </c>
@@ -10986,7 +11004,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>563</v>
       </c>
@@ -11024,7 +11042,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>442</v>
       </c>
@@ -11056,7 +11074,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>443</v>
       </c>
@@ -11088,7 +11106,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>434</v>
       </c>
@@ -11120,7 +11138,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>432</v>
       </c>
@@ -11152,7 +11170,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>428</v>
       </c>
@@ -11184,7 +11202,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>448</v>
       </c>
@@ -11216,7 +11234,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>436</v>
       </c>
@@ -11248,7 +11266,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>440</v>
       </c>
@@ -11280,7 +11298,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>382</v>
       </c>
@@ -11558,7 +11576,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>384</v>
       </c>
@@ -11593,7 +11611,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>701</v>
       </c>
@@ -11628,7 +11646,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>347</v>
       </c>
@@ -11663,7 +11681,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>351</v>
       </c>
@@ -11695,7 +11713,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>702</v>
       </c>
@@ -11730,7 +11748,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>569</v>
       </c>
@@ -11765,7 +11783,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>570</v>
       </c>
@@ -11896,7 +11914,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>390</v>
       </c>
@@ -11931,7 +11949,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>354</v>
       </c>
@@ -11969,7 +11987,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>450</v>
       </c>
@@ -12042,7 +12060,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>393</v>
       </c>
@@ -12077,7 +12095,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>552</v>
       </c>
@@ -12112,7 +12130,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>572</v>
       </c>
@@ -12147,7 +12165,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>573</v>
       </c>
@@ -12182,7 +12200,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>356</v>
       </c>
@@ -12217,7 +12235,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>359</v>
       </c>
@@ -12252,7 +12270,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>361</v>
       </c>
@@ -12287,15 +12305,15 @@
         <v>497</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>364</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>18</v>
+      <c r="C56" t="s">
+        <v>706</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>366</v>
@@ -12325,12 +12343,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>18</v>
+      <c r="C57" t="s">
+        <v>706</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>366</v>
@@ -12357,12 +12375,12 @@
         <v>498</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>18</v>
+      <c r="C58" t="s">
+        <v>706</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>366</v>
@@ -12427,7 +12445,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -12465,7 +12483,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>644</v>
       </c>
@@ -12503,7 +12521,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>640</v>
       </c>
@@ -12541,7 +12559,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>639</v>
       </c>
@@ -12579,7 +12597,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>705</v>
       </c>
@@ -12617,7 +12635,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>672</v>
       </c>
@@ -12655,7 +12673,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>370</v>
       </c>
@@ -12720,12 +12738,12 @@
         <v>497</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>18</v>
+      <c r="C68" t="s">
+        <v>706</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>366</v>
@@ -12759,7 +12777,7 @@
   <autoFilter ref="A1:M68" xr:uid="{3FE138CF-10D9-634A-87B2-6326254281CF}">
     <filterColumn colId="2">
       <filters>
-        <filter val="example-springboot"/>
+        <filter val="eo-test"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12914,11 +12932,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420FD413-96A0-5F4E-9C1C-71614BF4B061}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13066,6 +13084,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J5" xr:uid="{0C8B901F-485F-0747-B42C-E0000485C350}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V0.7.0 Refactored java builder with element calls
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/eo.xlsx
+++ b/builder/src/main/resources/eo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werner.diwischek/dev/elasticobjects/builder/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3CDF95-54C4-E34F-A725-8CECDD330BD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104D278D-975C-D742-9767-85D113337A1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="600" windowWidth="28240" windowHeight="17100" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
+    <workbookView xWindow="560" yWindow="900" windowWidth="28240" windowHeight="17100" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DbSqlConfig!$A$1:$I$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FieldConfig!$A$1:$J$125</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FileConfig!$A$1:$N$70</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ModelConfig!$A$1:$N$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ModelConfig!$A$1:$N$131</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="761">
   <si>
     <t>naturalId</t>
   </si>
@@ -2366,6 +2366,48 @@
   </si>
   <si>
     <t>CsvProperties,ListProperties</t>
+  </si>
+  <si>
+    <t>JavaFieldFinalCall</t>
+  </si>
+  <si>
+    <t>org.fluentcodes.projects.elasticobjects.calls.generate.java</t>
+  </si>
+  <si>
+    <t>Returns "final" string when final value is true.</t>
+  </si>
+  <si>
+    <t>JavaExtendsCall</t>
+  </si>
+  <si>
+    <t>Returns "extends" with superKey if superKey is not empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If type of the field is map, string or array a check for is empty is returned. </t>
+  </si>
+  <si>
+    <t>JavaFieldOverrideCall</t>
+  </si>
+  <si>
+    <t>Returns  an "@override" annotation is override field value is true.</t>
+  </si>
+  <si>
+    <t>JavaFieldTypeCall</t>
+  </si>
+  <si>
+    <t>Returns a type String depending on the modelKeys field value, e.g. "&lt;Map, AnObject&gt;" if modeKey is "Map, AnObject".</t>
+  </si>
+  <si>
+    <t>JavaImplementsCall</t>
+  </si>
+  <si>
+    <t>Returns the "implements " statement from the interfaces field value.</t>
+  </si>
+  <si>
+    <t>TreeMap</t>
+  </si>
+  <si>
+    <t>JavaFieldNotEmptyCall</t>
   </si>
 </sst>
 </file>
@@ -2751,13 +2793,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2949A4-7E1C-7F4B-A1BC-11445B521B01}">
-  <dimension ref="A1:O124"/>
+  <dimension ref="A1:O131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
+      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3132,7 +3174,7 @@
         <v>175</v>
       </c>
       <c r="L11" s="2" t="str">
-        <f>A11</f>
+        <f t="shared" ref="L11:L21" si="0">A11</f>
         <v>CallContent</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -3171,7 +3213,7 @@
         <v>175</v>
       </c>
       <c r="L12" s="2" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>CallImpl</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -3204,7 +3246,7 @@
         <v>175</v>
       </c>
       <c r="L13" s="2" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>CallKeep</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -3234,7 +3276,7 @@
         <v>173</v>
       </c>
       <c r="L14" s="2" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>Class</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -3264,7 +3306,7 @@
         <v>167</v>
       </c>
       <c r="L15" s="2" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>Condition</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -3300,7 +3342,7 @@
         <v>184</v>
       </c>
       <c r="L16" s="2" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>Config</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -3336,7 +3378,7 @@
         <v>187</v>
       </c>
       <c r="L17" s="2" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>ConfigAsFlatListCall</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -3372,7 +3414,7 @@
         <v>187</v>
       </c>
       <c r="L18" s="2" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>ConfigCall</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -3411,7 +3453,7 @@
         <v>184</v>
       </c>
       <c r="L19" s="2" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>ConfigImpl</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -3447,7 +3489,7 @@
         <v>187</v>
       </c>
       <c r="L20" s="2" t="str">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>ConfigKeysCall</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -3480,7 +3522,7 @@
         <v>212</v>
       </c>
       <c r="L21" s="2" t="str">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>ConfigLinkCall</v>
       </c>
       <c r="M21" s="2" t="s">
@@ -3837,7 +3879,7 @@
         <v>278</v>
       </c>
       <c r="L32" s="2" t="str">
-        <f>A32</f>
+        <f t="shared" ref="L32:L48" si="1">A32</f>
         <v>DbCall</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -3876,7 +3918,7 @@
         <v>278</v>
       </c>
       <c r="L33" s="2" t="str">
-        <f>A33</f>
+        <f t="shared" si="1"/>
         <v>DbConfig</v>
       </c>
       <c r="M33" s="2" t="s">
@@ -3909,7 +3951,7 @@
         <v>278</v>
       </c>
       <c r="L34" s="2" t="str">
-        <f>A34</f>
+        <f t="shared" si="1"/>
         <v>DbModelCall</v>
       </c>
       <c r="M34" s="2" t="s">
@@ -3942,7 +3984,7 @@
         <v>278</v>
       </c>
       <c r="L35" s="2" t="str">
-        <f>A35</f>
+        <f t="shared" si="1"/>
         <v>DbModelDeleteCall</v>
       </c>
       <c r="M35" s="2" t="s">
@@ -3978,7 +4020,7 @@
         <v>278</v>
       </c>
       <c r="L36" s="2" t="str">
-        <f>A36</f>
+        <f t="shared" si="1"/>
         <v>DbModelReadCall</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -4011,7 +4053,7 @@
         <v>278</v>
       </c>
       <c r="L37" s="2" t="str">
-        <f>A37</f>
+        <f t="shared" si="1"/>
         <v>DbModelWriteCall</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -4044,7 +4086,7 @@
         <v>278</v>
       </c>
       <c r="L38" s="2" t="str">
-        <f>A38</f>
+        <f t="shared" si="1"/>
         <v>DbProperties</v>
       </c>
       <c r="M38" s="2" t="s">
@@ -4080,7 +4122,7 @@
         <v>278</v>
       </c>
       <c r="L39" s="2" t="str">
-        <f>A39</f>
+        <f t="shared" si="1"/>
         <v>DbSqlCall</v>
       </c>
       <c r="M39" s="2" t="s">
@@ -4119,7 +4161,7 @@
         <v>278</v>
       </c>
       <c r="L40" s="2" t="str">
-        <f>A40</f>
+        <f t="shared" si="1"/>
         <v>DbSqlConfig</v>
       </c>
       <c r="M40" s="2" t="s">
@@ -4152,7 +4194,7 @@
         <v>278</v>
       </c>
       <c r="L41" s="2" t="str">
-        <f>A41</f>
+        <f t="shared" si="1"/>
         <v>DbSqlExecuteCall</v>
       </c>
       <c r="M41" s="2" t="s">
@@ -4185,7 +4227,7 @@
         <v>278</v>
       </c>
       <c r="L42" s="2" t="str">
-        <f>A42</f>
+        <f t="shared" si="1"/>
         <v>DbSqlProperties</v>
       </c>
       <c r="M42" s="2" t="s">
@@ -4221,7 +4263,7 @@
         <v>278</v>
       </c>
       <c r="L43" s="2" t="str">
-        <f>A43</f>
+        <f t="shared" si="1"/>
         <v>DbSqlReadCall</v>
       </c>
       <c r="M43" s="2" t="s">
@@ -4254,7 +4296,7 @@
         <v>278</v>
       </c>
       <c r="L44" s="2" t="str">
-        <f>A44</f>
+        <f t="shared" si="1"/>
         <v>DbTypes</v>
       </c>
       <c r="M44" s="2" t="s">
@@ -4287,7 +4329,7 @@
         <v>207</v>
       </c>
       <c r="L45" s="2" t="str">
-        <f>A45</f>
+        <f t="shared" si="1"/>
         <v>DirectoryConfig</v>
       </c>
       <c r="M45" s="2" t="s">
@@ -4320,7 +4362,7 @@
         <v>207</v>
       </c>
       <c r="L46" s="2" t="str">
-        <f>A46</f>
+        <f t="shared" si="1"/>
         <v>DirectoryListReadCall</v>
       </c>
       <c r="M46" s="2" t="s">
@@ -4356,7 +4398,7 @@
         <v>207</v>
       </c>
       <c r="L47" s="2" t="str">
-        <f>A47</f>
+        <f t="shared" si="1"/>
         <v>DirectoryMapReadCall</v>
       </c>
       <c r="M47" s="2" t="s">
@@ -4392,7 +4434,7 @@
         <v>207</v>
       </c>
       <c r="L48" s="2" t="str">
-        <f>A48</f>
+        <f t="shared" si="1"/>
         <v>DirectoryReadCall</v>
       </c>
       <c r="M48" s="2" t="s">
@@ -4785,7 +4827,7 @@
         <v>616</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>613</v>
+        <v>748</v>
       </c>
       <c r="L60" s="2" t="str">
         <f>A60</f>
@@ -4899,50 +4941,51 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L64" s="2" t="str">
+        <f>A64</f>
+        <v>TreeMap</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="C65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>707</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>691</v>
@@ -4951,51 +4994,54 @@
         <v>41</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>706</v>
+        <v>211</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="L65" s="2" t="str">
-        <f>A65</f>
-        <v>HostProperties</v>
+      <c r="L65" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>169</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>237</v>
+        <v>707</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>388</v>
+        <v>11</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>691</v>
+      </c>
       <c r="I66" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="J66" s="2" t="s">
+        <v>706</v>
+      </c>
       <c r="K66" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>81</v>
+        <v>175</v>
+      </c>
+      <c r="L66" s="2" t="str">
+        <f>A66</f>
+        <v>HostProperties</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>237</v>
@@ -5010,10 +5056,10 @@
         <v>41</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="M67" s="2" t="s">
         <v>460</v>
@@ -5021,31 +5067,32 @@
     </row>
     <row r="68" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>237</v>
+        <v>750</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="I68" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>216</v>
+        <v>751</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>92</v>
+        <v>748</v>
+      </c>
+      <c r="L68" s="2" t="str">
+        <f>A68</f>
+        <v>JavaExtendsCall</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>169</v>
@@ -5053,31 +5100,32 @@
     </row>
     <row r="69" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>217</v>
+        <v>747</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>181</v>
+      <c r="G69" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>218</v>
+        <v>749</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>217</v>
+        <v>748</v>
+      </c>
+      <c r="L69" s="2" t="str">
+        <f>A69</f>
+        <v>JavaFieldFinalCall</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>169</v>
@@ -5085,158 +5133,168 @@
     </row>
     <row r="70" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>231</v>
+        <v>760</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>388</v>
+        <v>343</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="I70" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>752</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>219</v>
+        <v>748</v>
+      </c>
+      <c r="L70" s="2" t="str">
+        <f>A70</f>
+        <v>JavaFieldNotEmptyCall</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>239</v>
+        <v>753</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G71" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="I71" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>754</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>220</v>
+        <v>748</v>
+      </c>
+      <c r="L71" s="2" t="str">
+        <f>A71</f>
+        <v>JavaFieldOverrideCall</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>229</v>
+        <v>755</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>388</v>
+        <v>343</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="I72" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>756</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>221</v>
+        <v>748</v>
+      </c>
+      <c r="L72" s="2" t="str">
+        <f>A72</f>
+        <v>JavaFieldTypeCall</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>391</v>
+        <v>757</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>390</v>
+      <c r="G73" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>434</v>
+        <v>758</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M73" s="5" t="s">
-        <v>461</v>
+        <v>748</v>
+      </c>
+      <c r="L73" s="2" t="str">
+        <f>A73</f>
+        <v>JavaImplementsCall</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="N73" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>97</v>
+        <v>139</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="I74" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J74" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="K74" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>224</v>
+        <v>92</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>11</v>
@@ -5244,34 +5302,28 @@
       <c r="D75" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>665</v>
-      </c>
       <c r="I75" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>435</v>
+        <v>216</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>224</v>
+        <v>92</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>431</v>
+        <v>217</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>11</v>
@@ -5280,36 +5332,33 @@
         <v>12</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>666</v>
+        <v>181</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>651</v>
+        <v>218</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>222</v>
+        <v>167</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>431</v>
+        <v>217</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>100</v>
+        <v>219</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>388</v>
@@ -5321,24 +5370,27 @@
         <v>41</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>100</v>
+        <v>219</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>460</v>
+        <v>470</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>237</v>
+        <v>220</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>388</v>
+        <v>11</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>12</v>
@@ -5347,18 +5399,24 @@
         <v>41</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>45</v>
+        <v>220</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>460</v>
+        <v>471</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>388</v>
@@ -5373,15 +5431,18 @@
         <v>170</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>227</v>
+        <v>391</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>11</v>
@@ -5389,34 +5450,31 @@
       <c r="D80" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>190</v>
+      <c r="E80" s="2" t="s">
+        <v>390</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>228</v>
+        <v>434</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>465</v>
+        <v>391</v>
+      </c>
+      <c r="M80" s="5" t="s">
+        <v>461</v>
       </c>
       <c r="N80" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>741</v>
+        <v>97</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>11</v>
@@ -5424,35 +5482,31 @@
       <c r="D81" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>235</v>
+      <c r="E81" s="2" t="s">
+        <v>390</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L81" s="2" t="str">
-        <f>A81</f>
-        <v>ModelConfigDbObject</v>
+        <v>222</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="N81" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>742</v>
+        <v>224</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>11</v>
@@ -5460,35 +5514,34 @@
       <c r="D82" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>743</v>
+      <c r="F82" s="2" t="s">
+        <v>391</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>591</v>
+        <v>665</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>709</v>
+        <v>435</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L82" s="2" t="str">
-        <f>A82</f>
-        <v>ModelConfigDbProperties</v>
+        <v>222</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>591</v>
+        <v>431</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>11</v>
@@ -5496,27 +5549,26 @@
       <c r="D83" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>475</v>
+      <c r="F83" s="2" t="s">
+        <v>391</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>183</v>
+        <v>666</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>228</v>
+        <v>651</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L83" s="2" t="str">
-        <f>A83</f>
-        <v>ModelConfigInterface</v>
+        <v>222</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>431</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="N83" s="2" t="s">
         <v>169</v>
@@ -5524,103 +5576,82 @@
     </row>
     <row r="84" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>229</v>
+        <v>100</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G84" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="I84" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J84" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="K84" s="2" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>229</v>
+        <v>100</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="N84" s="2" t="s">
-        <v>169</v>
+        <v>460</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>231</v>
+        <v>45</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G85" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="I85" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J85" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="K85" s="2" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>231</v>
+        <v>45</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="N85" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G86" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="I86" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J86" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="K86" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="N86" s="2" t="s">
-        <v>169</v>
+        <v>470</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>11</v>
@@ -5628,20 +5659,23 @@
       <c r="D87" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F87" s="2" t="s">
+        <v>708</v>
+      </c>
       <c r="G87" s="2" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="M87" s="2" t="s">
         <v>465</v>
@@ -5650,9 +5684,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>708</v>
+        <v>741</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>11</v>
@@ -5660,35 +5694,35 @@
       <c r="D88" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>744</v>
+      <c r="F88" s="2" t="s">
+        <v>745</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>591</v>
+        <v>235</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>709</v>
+        <v>236</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L88" s="2" t="str">
         <f>A88</f>
-        <v>ModelConfigProperties</v>
+        <v>ModelConfigDbObject</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>237</v>
+        <v>742</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>11</v>
@@ -5696,31 +5730,35 @@
       <c r="D89" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E89" s="2" t="s">
+        <v>743</v>
+      </c>
       <c r="G89" s="2" t="s">
-        <v>227</v>
+        <v>591</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>238</v>
+        <v>709</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="L89" s="2" t="s">
-        <v>237</v>
+      <c r="L89" s="2" t="str">
+        <f>A89</f>
+        <v>ModelConfigDbProperties</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="N89" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>239</v>
+        <v>591</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>11</v>
@@ -5728,23 +5766,27 @@
       <c r="D90" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E90" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G90" s="2" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="L90" s="2" t="s">
-        <v>239</v>
+      <c r="L90" s="2" t="str">
+        <f>A90</f>
+        <v>ModelConfigInterface</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="N90" s="2" t="s">
         <v>169</v>
@@ -5752,7 +5794,7 @@
     </row>
     <row r="91" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>11</v>
@@ -5760,17 +5802,20 @@
       <c r="D91" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G91" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="I91" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>465</v>
@@ -5781,57 +5826,63 @@
     </row>
     <row r="92" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B92" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="N92" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="M92" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="N92" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C93" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="I93" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>64</v>
+        <v>233</v>
       </c>
       <c r="M93" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>169</v>
@@ -5839,7 +5890,7 @@
     </row>
     <row r="94" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>11</v>
@@ -5847,28 +5898,31 @@
       <c r="D94" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="I94" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="N94" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>246</v>
+        <v>708</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>11</v>
@@ -5877,30 +5931,34 @@
         <v>12</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>285</v>
+        <v>744</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>591</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>247</v>
+        <v>709</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="L95" s="2" t="s">
-        <v>246</v>
+        <v>184</v>
+      </c>
+      <c r="L95" s="2" t="str">
+        <f>A95</f>
+        <v>ModelConfigProperties</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>692</v>
+        <v>237</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>11</v>
@@ -5908,24 +5966,23 @@
       <c r="D96" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>286</v>
+      <c r="G96" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L96" s="2" t="str">
-        <f>A96</f>
-        <v>PermissionRole</v>
+        <v>184</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>169</v>
@@ -5933,7 +5990,7 @@
     </row>
     <row r="97" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>664</v>
+        <v>239</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>11</v>
@@ -5941,30 +5998,23 @@
       <c r="D97" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>676</v>
-      </c>
       <c r="G97" s="2" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L97" s="2" t="str">
-        <f>A97</f>
-        <v>ResourceCall</v>
+        <v>184</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="N97" s="2" t="s">
         <v>169</v>
@@ -5972,7 +6022,7 @@
     </row>
     <row r="98" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>691</v>
+        <v>241</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>11</v>
@@ -5980,32 +6030,31 @@
       <c r="D98" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="I98" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L98" s="2" t="str">
-        <f>A98</f>
-        <v>ResourceConfig</v>
+        <v>184</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="M98" s="2" t="s">
         <v>465</v>
       </c>
+      <c r="N98" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="99" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>740</v>
+        <v>153</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>11</v>
@@ -6013,29 +6062,25 @@
       <c r="D99" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>695</v>
-      </c>
       <c r="I99" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J99" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="K99" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L99" s="2" t="str">
-        <f>A99</f>
-        <v>PermissionProperties</v>
+        <v>173</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="M99" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>665</v>
+        <v>64</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>11</v>
@@ -6043,27 +6088,20 @@
       <c r="D100" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>664</v>
-      </c>
       <c r="I100" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>667</v>
+        <v>243</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L100" s="2" t="str">
-        <f>A100</f>
-        <v>ResourceReadCall</v>
+        <v>167</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="M100" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="N100" s="2" t="s">
         <v>169</v>
@@ -6071,7 +6109,7 @@
     </row>
     <row r="101" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>666</v>
+        <v>244</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>11</v>
@@ -6079,30 +6117,20 @@
       <c r="D101" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>664</v>
-      </c>
       <c r="I101" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>668</v>
+        <v>245</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L101" s="2" t="str">
-        <f>A101</f>
-        <v>ResourceWriteCall</v>
+        <v>214</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="N101" s="2" t="s">
         <v>169</v>
@@ -6110,10 +6138,7 @@
     </row>
     <row r="102" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>11</v>
@@ -6121,20 +6146,23 @@
       <c r="D102" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E102" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="I102" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M102" s="2" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="N102" s="2" t="s">
         <v>169</v>
@@ -6142,10 +6170,7 @@
     </row>
     <row r="103" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>239</v>
+        <v>692</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>11</v>
@@ -6153,28 +6178,32 @@
       <c r="D103" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E103" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="I103" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="J103" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="K103" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>252</v>
+        <v>175</v>
+      </c>
+      <c r="L103" s="2" t="str">
+        <f t="shared" ref="L103:L108" si="2">A103</f>
+        <v>PermissionRole</v>
       </c>
       <c r="M103" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>237</v>
+        <v>664</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>11</v>
@@ -6182,20 +6211,30 @@
       <c r="D104" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E104" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="I104" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>253</v>
+        <v>179</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L104" s="2" t="s">
-        <v>144</v>
+        <v>175</v>
+      </c>
+      <c r="L104" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>ResourceCall</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>169</v>
@@ -6203,10 +6242,7 @@
     </row>
     <row r="105" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>237</v>
+        <v>691</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>11</v>
@@ -6214,25 +6250,32 @@
       <c r="D105" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F105" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="I105" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="J105" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="K105" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L105" s="2" t="s">
-        <v>254</v>
+        <v>175</v>
+      </c>
+      <c r="L105" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>ResourceConfig</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="N105" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>213</v>
+        <v>740</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>11</v>
@@ -6240,31 +6283,29 @@
       <c r="D106" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G106" s="2" t="s">
-        <v>177</v>
+      <c r="E106" s="2" t="s">
+        <v>695</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>255</v>
+        <v>195</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>213</v>
+        <v>175</v>
+      </c>
+      <c r="L106" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>PermissionProperties</v>
       </c>
       <c r="M106" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>256</v>
+        <v>665</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>11</v>
@@ -6272,23 +6313,27 @@
       <c r="D107" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E107" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="G107" s="2" t="s">
-        <v>177</v>
+        <v>664</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>257</v>
+        <v>667</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>256</v>
+        <v>175</v>
+      </c>
+      <c r="L107" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>ResourceReadCall</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>169</v>
@@ -6296,33 +6341,46 @@
     </row>
     <row r="108" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>237</v>
+        <v>666</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>388</v>
+        <v>11</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E108" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>664</v>
+      </c>
       <c r="I108" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="J108" s="2" t="s">
+        <v>668</v>
+      </c>
       <c r="K108" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>15</v>
+        <v>175</v>
+      </c>
+      <c r="L108" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>ResourceWriteCall</v>
       </c>
       <c r="M108" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>237</v>
@@ -6336,25 +6394,28 @@
       <c r="I109" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="J109" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="K109" s="2" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="M109" s="2" t="s">
         <v>463</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>11</v>
@@ -6366,21 +6427,24 @@
         <v>41</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="M110" s="2" t="s">
-        <v>463</v>
+        <v>474</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>260</v>
+        <v>144</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>11</v>
@@ -6388,31 +6452,31 @@
       <c r="D111" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G111" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="I111" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>260</v>
+        <v>144</v>
       </c>
       <c r="M111" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>11</v>
@@ -6420,35 +6484,26 @@
       <c r="D112" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G112" s="2" t="s">
+      <c r="I112" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L112" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="M112" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="N112" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="I112" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="K112" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="L112" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="M112" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="N112" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>491</v>
-      </c>
       <c r="C113" s="2" t="s">
         <v>11</v>
       </c>
@@ -6456,19 +6511,19 @@
         <v>12</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>490</v>
+        <v>255</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>212</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>491</v>
+        <v>213</v>
       </c>
       <c r="M113" s="2" t="s">
         <v>464</v>
@@ -6479,7 +6534,7 @@
     </row>
     <row r="114" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>497</v>
+        <v>256</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>11</v>
@@ -6488,19 +6543,19 @@
         <v>12</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>490</v>
+        <v>257</v>
       </c>
       <c r="K114" s="2" t="s">
         <v>212</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>497</v>
+        <v>256</v>
       </c>
       <c r="M114" s="2" t="s">
         <v>464</v>
@@ -6509,41 +6564,38 @@
         <v>169</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>264</v>
+        <v>15</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G115" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="I115" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>265</v>
+        <v>41</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>264</v>
+        <v>15</v>
       </c>
       <c r="M115" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="N115" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>11</v>
@@ -6551,31 +6603,28 @@
       <c r="D116" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G116" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="I116" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>265</v>
+        <v>41</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M116" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>11</v>
@@ -6583,38 +6632,25 @@
       <c r="D117" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="I117" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>268</v>
+        <v>41</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L117" s="2" t="str">
-        <f>A117</f>
-        <v>TemplateCall</v>
+        <v>173</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="M117" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>658</v>
+        <v>260</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>11</v>
@@ -6622,24 +6658,20 @@
       <c r="D118" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>663</v>
-      </c>
       <c r="G118" s="2" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>659</v>
+        <v>261</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L118" s="2" t="str">
-        <f>A118</f>
-        <v>TemplateDirResourceCall</v>
+        <v>212</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="M118" s="2" t="s">
         <v>464</v>
@@ -6648,9 +6680,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>11</v>
@@ -6659,26 +6691,22 @@
         <v>12</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>676</v>
+        <v>384</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>267</v>
+        <v>213</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>660</v>
+        <v>263</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L119" s="2" t="str">
-        <f>A119</f>
-        <v>TemplateResourceCall</v>
+        <v>212</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="M119" s="2" t="s">
         <v>464</v>
@@ -6687,9 +6715,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>11</v>
@@ -6697,24 +6725,20 @@
       <c r="D120" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="G120" s="2" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>270</v>
+        <v>490</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L120" s="2" t="str">
-        <f>A120</f>
-        <v>TemplateResourceStoreCall</v>
+        <v>212</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>491</v>
       </c>
       <c r="M120" s="2" t="s">
         <v>464</v>
@@ -6725,16 +6749,13 @@
     </row>
     <row r="121" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>287</v>
+        <v>497</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>288</v>
+        <v>11</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>213</v>
@@ -6743,14 +6764,13 @@
         <v>17</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>289</v>
+        <v>490</v>
       </c>
       <c r="K121" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="L121" s="2" t="str">
-        <f>A121</f>
-        <v>TheGreetingCall</v>
+      <c r="L121" s="2" t="s">
+        <v>497</v>
       </c>
       <c r="M121" s="2" t="s">
         <v>464</v>
@@ -6759,9 +6779,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>11</v>
@@ -6769,23 +6789,20 @@
       <c r="D122" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>674</v>
-      </c>
       <c r="G122" s="2" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>212</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="M122" s="2" t="s">
         <v>464</v>
@@ -6794,65 +6811,69 @@
         <v>169</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>417</v>
+        <v>11</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="G123" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="M123" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>417</v>
+        <v>11</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E124" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>674</v>
+      </c>
       <c r="G124" s="2" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>652</v>
+        <v>268</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="L124" s="2" t="s">
-        <v>293</v>
+        <v>215</v>
+      </c>
+      <c r="L124" s="2" t="str">
+        <f>A124</f>
+        <v>TemplateCall</v>
       </c>
       <c r="M124" s="2" t="s">
         <v>464</v>
@@ -6861,14 +6882,263 @@
         <v>169</v>
       </c>
     </row>
+    <row r="125" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L125" s="2" t="str">
+        <f>A125</f>
+        <v>TemplateDirResourceCall</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L126" s="2" t="str">
+        <f>A126</f>
+        <v>TemplateResourceCall</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I127" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L127" s="2" t="str">
+        <f>A127</f>
+        <v>TemplateResourceStoreCall</v>
+      </c>
+      <c r="M127" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N127" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I128" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="K128" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L128" s="2" t="str">
+        <f>A128</f>
+        <v>TheGreetingCall</v>
+      </c>
+      <c r="M128" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I129" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="K129" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="M129" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M130" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="N130" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K131" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="L131" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="M131" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N131" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N124" xr:uid="{A955F0F7-5ED5-4A4E-94AE-7EA930688524}">
-    <sortState ref="A2:N124">
-      <sortCondition ref="A2:A124"/>
+  <autoFilter ref="A1:N131" xr:uid="{A955F0F7-5ED5-4A4E-94AE-7EA930688524}">
+    <sortState ref="A2:N131">
+      <sortCondition ref="A2:A131"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:N124">
-    <sortCondition ref="A2:A124"/>
+  <sortState ref="A2:N131">
+    <sortCondition ref="A2:A131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8126,7 +8396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -8177,7 +8447,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -8198,7 +8468,7 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="str">
-        <f>A49</f>
+        <f t="shared" ref="H49:H57" si="0">A49</f>
         <v>interfaces</v>
       </c>
       <c r="I49">
@@ -8225,11 +8495,11 @@
         <v>41</v>
       </c>
       <c r="H50" t="str">
-        <f>A50</f>
+        <f t="shared" si="0"/>
         <v>javaProperties</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>305</v>
       </c>
@@ -8250,14 +8520,14 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="str">
-        <f>A51</f>
+        <f t="shared" si="0"/>
         <v>jndi</v>
       </c>
       <c r="I51">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -8278,14 +8548,14 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="str">
-        <f>A52</f>
+        <f t="shared" si="0"/>
         <v>join</v>
       </c>
       <c r="I52">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -8305,14 +8575,14 @@
         <v>41</v>
       </c>
       <c r="H53" t="str">
-        <f>A53</f>
+        <f t="shared" si="0"/>
         <v>joinInverse</v>
       </c>
       <c r="I53">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -8333,7 +8603,7 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="str">
-        <f>A54</f>
+        <f t="shared" si="0"/>
         <v>keepCall</v>
       </c>
     </row>
@@ -8358,7 +8628,7 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="str">
-        <f>A55</f>
+        <f t="shared" si="0"/>
         <v>key</v>
       </c>
       <c r="I55">
@@ -8386,11 +8656,11 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="str">
-        <f>A56</f>
+        <f t="shared" si="0"/>
         <v>length</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -8411,14 +8681,14 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="str">
-        <f>A57</f>
+        <f t="shared" si="0"/>
         <v>listParams</v>
       </c>
       <c r="I57">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>424</v>
       </c>
@@ -8468,7 +8738,7 @@
         <v>logLevel</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -8496,7 +8766,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -8551,7 +8821,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -8578,7 +8848,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -8602,7 +8872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>109</v>
       </c>
@@ -8629,7 +8899,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -8656,7 +8926,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>449</v>
       </c>
@@ -8704,7 +8974,7 @@
       </c>
       <c r="G68" s="1"/>
       <c r="H68" t="str">
-        <f>A68</f>
+        <f t="shared" ref="H68:H81" si="1">A68</f>
         <v>myAnObject</v>
       </c>
     </row>
@@ -8730,7 +9000,7 @@
       </c>
       <c r="G69" s="1"/>
       <c r="H69" t="str">
-        <f>A69</f>
+        <f t="shared" si="1"/>
         <v>myASubObject</v>
       </c>
     </row>
@@ -8755,7 +9025,7 @@
       </c>
       <c r="G70" s="1"/>
       <c r="H70" t="str">
-        <f>A70</f>
+        <f t="shared" si="1"/>
         <v>myASubObjectList</v>
       </c>
     </row>
@@ -8780,7 +9050,7 @@
       </c>
       <c r="G71" s="1"/>
       <c r="H71" t="str">
-        <f>A71</f>
+        <f t="shared" si="1"/>
         <v>myASubObjectMap</v>
       </c>
     </row>
@@ -8798,7 +9068,7 @@
         <v>19</v>
       </c>
       <c r="E72" s="1" t="str">
-        <f>A72</f>
+        <f t="shared" ref="E72:E79" si="2">A72</f>
         <v>myBoolean</v>
       </c>
       <c r="F72" t="s">
@@ -8806,7 +9076,7 @@
       </c>
       <c r="G72" s="1"/>
       <c r="H72" t="str">
-        <f>A72</f>
+        <f t="shared" si="1"/>
         <v>myBoolean</v>
       </c>
     </row>
@@ -8824,7 +9094,7 @@
         <v>36</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>A73</f>
+        <f t="shared" si="2"/>
         <v>myDate</v>
       </c>
       <c r="F73" t="s">
@@ -8832,7 +9102,7 @@
       </c>
       <c r="G73" s="1"/>
       <c r="H73" t="str">
-        <f>A73</f>
+        <f t="shared" si="1"/>
         <v>myDate</v>
       </c>
     </row>
@@ -8850,7 +9120,7 @@
         <v>151</v>
       </c>
       <c r="E74" s="1" t="str">
-        <f>A74</f>
+        <f t="shared" si="2"/>
         <v>myDouble</v>
       </c>
       <c r="F74" t="s">
@@ -8858,7 +9128,7 @@
       </c>
       <c r="G74" s="1"/>
       <c r="H74" t="str">
-        <f>A74</f>
+        <f t="shared" si="1"/>
         <v>myDouble</v>
       </c>
     </row>
@@ -8876,7 +9146,7 @@
         <v>152</v>
       </c>
       <c r="E75" s="1" t="str">
-        <f>A75</f>
+        <f t="shared" si="2"/>
         <v>myFloat</v>
       </c>
       <c r="F75" t="s">
@@ -8884,7 +9154,7 @@
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="str">
-        <f>A75</f>
+        <f t="shared" si="1"/>
         <v>myFloat</v>
       </c>
     </row>
@@ -8902,14 +9172,14 @@
         <v>81</v>
       </c>
       <c r="E76" s="1" t="str">
-        <f>A76</f>
+        <f t="shared" si="2"/>
         <v>myInt</v>
       </c>
       <c r="F76" t="s">
         <v>17</v>
       </c>
       <c r="H76" t="str">
-        <f>A76</f>
+        <f t="shared" si="1"/>
         <v>myInt</v>
       </c>
     </row>
@@ -8927,7 +9197,7 @@
         <v>48</v>
       </c>
       <c r="E77" s="1" t="str">
-        <f>A77</f>
+        <f t="shared" si="2"/>
         <v>myList</v>
       </c>
       <c r="F77" t="s">
@@ -8935,7 +9205,7 @@
       </c>
       <c r="G77" s="1"/>
       <c r="H77" t="str">
-        <f>A77</f>
+        <f t="shared" si="1"/>
         <v>myList</v>
       </c>
     </row>
@@ -8953,7 +9223,7 @@
         <v>45</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>A78</f>
+        <f t="shared" si="2"/>
         <v>myLong</v>
       </c>
       <c r="F78" t="s">
@@ -8961,7 +9231,7 @@
       </c>
       <c r="G78" s="1"/>
       <c r="H78" t="str">
-        <f>A78</f>
+        <f t="shared" si="1"/>
         <v>myLong</v>
       </c>
     </row>
@@ -8979,14 +9249,14 @@
         <v>38</v>
       </c>
       <c r="E79" s="1" t="str">
-        <f>A79</f>
+        <f t="shared" si="2"/>
         <v>myMap</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
       </c>
       <c r="H79" t="str">
-        <f>A79</f>
+        <f t="shared" si="1"/>
         <v>myMap</v>
       </c>
     </row>
@@ -9011,11 +9281,11 @@
       </c>
       <c r="G80" s="1"/>
       <c r="H80" t="str">
-        <f>A80</f>
+        <f t="shared" si="1"/>
         <v>myObject</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>512</v>
       </c>
@@ -9036,7 +9306,7 @@
       </c>
       <c r="G81" s="1"/>
       <c r="H81" t="str">
-        <f>A81</f>
+        <f t="shared" si="1"/>
         <v>myString</v>
       </c>
       <c r="I81">
@@ -9524,7 +9794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>131</v>
       </c>
@@ -9701,7 +9971,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>141</v>
       </c>
@@ -9780,7 +10050,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>145</v>
       </c>
@@ -9834,7 +10104,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>311</v>
       </c>
@@ -9886,7 +10156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>559</v>
       </c>
@@ -9913,7 +10183,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>146</v>
       </c>
@@ -9940,7 +10210,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>148</v>
       </c>
@@ -9967,7 +10237,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>486</v>
       </c>
@@ -9994,7 +10264,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>150</v>
       </c>
@@ -10180,7 +10450,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>164</v>
       </c>
@@ -13364,7 +13634,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>372</v>
       </c>

</xml_diff>